<commit_message>
Added data sheet TC-55056
</commit_message>
<xml_diff>
--- a/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
+++ b/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="TC_55046" sheetId="1" r:id="rId1"/>
     <sheet name="TC_55052" sheetId="3" r:id="rId2"/>
+    <sheet name="TC_55056" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -141,6 +142,48 @@
   </si>
   <si>
     <t>P80AV - R/W - 3</t>
+  </si>
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Parameter added</t>
+  </si>
+  <si>
+    <t>S-BOXR Shallow box wallsdr Red</t>
+  </si>
+  <si>
+    <t>S-BOXW Shallow box wallsdr White</t>
+  </si>
+  <si>
+    <t>P80AI - R/W  - 5</t>
+  </si>
+  <si>
+    <t>P80AV - R/W - 7</t>
+  </si>
+  <si>
+    <t>D-BOXW Deep box wallsdr White</t>
+  </si>
+  <si>
+    <t>D-BOXR Deep box wallsdr Red</t>
+  </si>
+  <si>
+    <t>557.080.007</t>
+  </si>
+  <si>
+    <t>557.080.008</t>
+  </si>
+  <si>
+    <t>557.080.011</t>
+  </si>
+  <si>
+    <t>557.080.012</t>
+  </si>
+  <si>
+    <t>Surface Box</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -241,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -258,13 +301,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,13 +638,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -606,11 +653,11 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -690,7 +737,7 @@
       <c r="F8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -716,7 +763,7 @@
       <c r="F9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -742,7 +789,7 @@
       <c r="F10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -768,7 +815,7 @@
       <c r="F11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -789,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,16 +848,17 @@
     <col min="4" max="4" width="37.21875" customWidth="1"/>
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -820,11 +868,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -894,7 +942,9 @@
       <c r="G7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
     </row>
@@ -917,10 +967,12 @@
       <c r="F8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
     </row>
@@ -943,10 +995,12 @@
       <c r="F9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
@@ -1006,4 +1060,184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data sheet NGC-1345 updated
</commit_message>
<xml_diff>
--- a/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
+++ b/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_55046" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>P80AI - R/W</t>
-  </si>
-  <si>
     <t>P80AV - R/W</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">P80AI - R/W </t>
   </si>
 </sst>
 </file>
@@ -302,15 +302,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,13 +638,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -653,11 +653,11 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -738,7 +738,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>32</v>
@@ -764,7 +764,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>32</v>
@@ -790,7 +790,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>32</v>
@@ -816,7 +816,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>32</v>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,13 +852,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -868,11 +868,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -950,56 +950,56 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>55</v>
+        <v>34</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>55</v>
+        <v>34</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,24 +1081,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1140,10 +1140,10 @@
         <v>13</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>26</v>
@@ -1151,87 +1151,87 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="15"/>
+        <v>49</v>
+      </c>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="G11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1239,5 +1239,6 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data sheet NGC-1345
</commit_message>
<xml_diff>
--- a/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
+++ b/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC_55046" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t xml:space="preserve">P80AI - R/W </t>
+  </si>
+  <si>
+    <t>Status In B</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +640,7 @@
     <col min="11" max="11" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -646,7 +649,7 @@
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -659,7 +662,7 @@
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -672,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,14 +688,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -717,8 +720,11 @@
       <c r="H7" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -743,8 +749,11 @@
       <c r="H8" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -769,8 +778,11 @@
       <c r="H9" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -795,8 +807,11 @@
       <c r="H10" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
@@ -819,6 +834,9 @@
         <v>34</v>
       </c>
       <c r="H11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -836,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,7 +963,9 @@
       <c r="H7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="11"/>
+      <c r="I7" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -973,7 +993,9 @@
       <c r="H8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11"/>
+      <c r="I8" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1001,7 +1023,9 @@
       <c r="H9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1066,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Test data sheets TC-55046, TC-64
</commit_message>
<xml_diff>
--- a/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
+++ b/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_55046" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,8 +775,8 @@
       <c r="G9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>32</v>
+      <c r="H9" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>32</v>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,8 +990,8 @@
       <c r="G8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>54</v>
+      <c r="H8" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>32</v>
@@ -1020,8 +1020,8 @@
       <c r="G9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>54</v>
+      <c r="H9" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>32</v>
@@ -1090,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data sheets TC-55052 and Multiple point wizard NGC-1826
</commit_message>
<xml_diff>
--- a/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
+++ b/Test Data/TC_55046_55052_55056_Verify_Combobox_And_Shopping_List.xlsx
@@ -852,10 +852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,54 +1027,6 @@
         <v>32</v>
       </c>
       <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>